<commit_message>
correction to Asn flux
</commit_message>
<xml_diff>
--- a/H1299_143B_prot-nucl-quant/Asn-consumption-flux_143B/output/influx.xlsx
+++ b/H1299_143B_prot-nucl-quant/Asn-consumption-flux_143B/output/influx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Sample_name</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Arginine pos</t>
-  </si>
-  <si>
-    <t>Asparagine pos</t>
   </si>
   <si>
     <t>Asparagine-13C4 pos</t>
@@ -506,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,13 +570,10 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" t="s">
-        <v>21</v>
       </c>
       <c r="B2">
         <v>24</v>
@@ -638,13 +632,10 @@
       <c r="T2">
         <v>0</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>24</v>
@@ -703,13 +694,10 @@
       <c r="T3">
         <v>0</v>
       </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -768,13 +756,10 @@
       <c r="T4">
         <v>0</v>
       </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -833,13 +818,10 @@
       <c r="T5">
         <v>0</v>
       </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>24</v>
@@ -898,13 +880,10 @@
       <c r="T6">
         <v>0</v>
       </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>24</v>
@@ -963,79 +942,76 @@
       <c r="T7">
         <v>0</v>
       </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" t="s">
         <v>32</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" t="s">
-        <v>33</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -1050,57 +1026,54 @@
         <v>3.748523063341041</v>
       </c>
       <c r="F14">
-        <v>-0.5970038421498086</v>
+        <v>3.038633187518536</v>
       </c>
       <c r="G14">
-        <v>2.441629345368727</v>
+        <v>-0.1363927765851398</v>
       </c>
       <c r="H14">
-        <v>-0.1363927765851398</v>
+        <v>-11.95938718794047</v>
       </c>
       <c r="I14">
-        <v>-11.95938718794047</v>
+        <v>59.98559571372608</v>
       </c>
       <c r="J14">
-        <v>59.98559571372608</v>
+        <v>5.247950854503589</v>
       </c>
       <c r="K14">
-        <v>5.247950854503589</v>
+        <v>13.58518841594817</v>
       </c>
       <c r="L14">
-        <v>13.58518841594817</v>
+        <v>3.210392764755202</v>
       </c>
       <c r="M14">
-        <v>3.210392764755202</v>
+        <v>1.61180319428877</v>
       </c>
       <c r="N14">
-        <v>1.61180319428877</v>
+        <v>1.206780652774268</v>
       </c>
       <c r="O14">
-        <v>1.206780652774268</v>
+        <v>-0.2735792296196853</v>
       </c>
       <c r="P14">
-        <v>-0.2735792296196853</v>
+        <v>4.929303332391661</v>
       </c>
       <c r="Q14">
-        <v>4.929303332391661</v>
+        <v>-1.134159218312993</v>
       </c>
       <c r="R14">
-        <v>-1.134159218312993</v>
+        <v>0.4299133804864244</v>
       </c>
       <c r="S14">
-        <v>0.4299133804864244</v>
+        <v>1.697147275545372</v>
       </c>
       <c r="T14">
-        <v>1.697147275545372</v>
-      </c>
-      <c r="U14">
         <v>1.842962743725967</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -1115,57 +1088,54 @@
         <v>3.076128578302698</v>
       </c>
       <c r="F15">
-        <v>-0.4958221547328643</v>
+        <v>2.243094108572594</v>
       </c>
       <c r="G15">
-        <v>1.747271953839729</v>
+        <v>-0.116911282264837</v>
       </c>
       <c r="H15">
-        <v>-0.116911282264837</v>
+        <v>-12.30000853315675</v>
       </c>
       <c r="I15">
-        <v>-12.30000853315675</v>
+        <v>62.99746892220585</v>
       </c>
       <c r="J15">
-        <v>62.99746892220585</v>
+        <v>8.965055196193971</v>
       </c>
       <c r="K15">
-        <v>8.965055196193971</v>
+        <v>6.065302642228615</v>
       </c>
       <c r="L15">
-        <v>6.065302642228615</v>
+        <v>2.801894800216087</v>
       </c>
       <c r="M15">
-        <v>2.801894800216087</v>
+        <v>0.8688306563646487</v>
       </c>
       <c r="N15">
-        <v>0.8688306563646487</v>
+        <v>2.256192149327042</v>
       </c>
       <c r="O15">
-        <v>2.256192149327042</v>
+        <v>-0.2737328060678731</v>
       </c>
       <c r="P15">
-        <v>-0.2737328060678731</v>
+        <v>5.587459923675186</v>
       </c>
       <c r="Q15">
-        <v>5.587459923675186</v>
+        <v>0.6647825856250542</v>
       </c>
       <c r="R15">
-        <v>0.6647825856250542</v>
+        <v>0.4260476910267606</v>
       </c>
       <c r="S15">
-        <v>0.4260476910267606</v>
+        <v>1.32384942745239</v>
       </c>
       <c r="T15">
-        <v>1.32384942745239</v>
-      </c>
-      <c r="U15">
         <v>0.8163445185513934</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -1180,57 +1150,54 @@
         <v>3.632028168871455</v>
       </c>
       <c r="F16">
-        <v>-0.4753368213480372</v>
+        <v>2.068234961241354</v>
       </c>
       <c r="G16">
-        <v>1.592898139893317</v>
+        <v>-0.118906790336939</v>
       </c>
       <c r="H16">
-        <v>-0.118906790336939</v>
+        <v>-12.62724723881968</v>
       </c>
       <c r="I16">
-        <v>-12.62724723881968</v>
+        <v>61.40410858476258</v>
       </c>
       <c r="J16">
-        <v>61.40410858476258</v>
+        <v>4.850980607828805</v>
       </c>
       <c r="K16">
-        <v>4.850980607828805</v>
+        <v>12.52787090650216</v>
       </c>
       <c r="L16">
-        <v>12.52787090650216</v>
+        <v>5.115208632647017</v>
       </c>
       <c r="M16">
-        <v>5.115208632647017</v>
+        <v>1.04629502649541</v>
       </c>
       <c r="N16">
-        <v>1.04629502649541</v>
+        <v>1.414475268520692</v>
       </c>
       <c r="O16">
-        <v>1.414475268520692</v>
+        <v>-0.2622822292035848</v>
       </c>
       <c r="P16">
-        <v>-0.2622822292035848</v>
+        <v>4.736694917501496</v>
       </c>
       <c r="Q16">
-        <v>4.736694917501496</v>
+        <v>-2.687975518517275</v>
       </c>
       <c r="R16">
-        <v>-2.687975518517275</v>
+        <v>0.3654975397701379</v>
       </c>
       <c r="S16">
-        <v>0.3654975397701379</v>
+        <v>1.42611402880803</v>
       </c>
       <c r="T16">
-        <v>1.42611402880803</v>
-      </c>
-      <c r="U16">
         <v>4.615967092588386</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -1245,57 +1212,54 @@
         <v>3.961007909887437</v>
       </c>
       <c r="F17">
-        <v>-0.5745077979883825</v>
+        <v>2.976720607509004</v>
       </c>
       <c r="G17">
-        <v>2.402212809520622</v>
+        <v>-0.09487548699717202</v>
       </c>
       <c r="H17">
-        <v>-0.09487548699717202</v>
+        <v>-12.13244655958362</v>
       </c>
       <c r="I17">
-        <v>-12.13244655958362</v>
+        <v>61.42082797863986</v>
       </c>
       <c r="J17">
-        <v>61.42082797863986</v>
+        <v>-2.930068659938121</v>
       </c>
       <c r="K17">
-        <v>-2.930068659938121</v>
+        <v>20.74242844474741</v>
       </c>
       <c r="L17">
-        <v>20.74242844474741</v>
+        <v>5.369760005481086</v>
       </c>
       <c r="M17">
-        <v>5.369760005481086</v>
+        <v>1.340042046655768</v>
       </c>
       <c r="N17">
-        <v>1.340042046655768</v>
+        <v>1.554605892041782</v>
       </c>
       <c r="O17">
-        <v>1.554605892041782</v>
+        <v>-0.2601983872813319</v>
       </c>
       <c r="P17">
-        <v>-0.2601983872813319</v>
+        <v>5.679047349473693</v>
       </c>
       <c r="Q17">
-        <v>5.679047349473693</v>
+        <v>2.534304179205914</v>
       </c>
       <c r="R17">
-        <v>2.534304179205914</v>
+        <v>0.6572937031741428</v>
       </c>
       <c r="S17">
-        <v>0.6572937031741428</v>
+        <v>0.9363639784668653</v>
       </c>
       <c r="T17">
-        <v>0.9363639784668653</v>
-      </c>
-      <c r="U17">
         <v>7.291485154995129</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -1310,57 +1274,54 @@
         <v>3.981324865599323</v>
       </c>
       <c r="F18">
-        <v>-0.3961669412943233</v>
+        <v>2.225486338339457</v>
       </c>
       <c r="G18">
-        <v>1.829319397045134</v>
+        <v>-0.1197414778538239</v>
       </c>
       <c r="H18">
-        <v>-0.1197414778538239</v>
+        <v>-12.23476239431361</v>
       </c>
       <c r="I18">
-        <v>-12.23476239431361</v>
+        <v>74.1565300753155</v>
       </c>
       <c r="J18">
-        <v>74.1565300753155</v>
+        <v>21.9110401291382</v>
       </c>
       <c r="K18">
-        <v>21.9110401291382</v>
+        <v>-5.573269248576242</v>
       </c>
       <c r="L18">
-        <v>-5.573269248576242</v>
+        <v>4.548303101827099</v>
       </c>
       <c r="M18">
-        <v>4.548303101827099</v>
+        <v>1.629712951467569</v>
       </c>
       <c r="N18">
-        <v>1.629712951467569</v>
+        <v>2.088035511962444</v>
       </c>
       <c r="O18">
-        <v>2.088035511962444</v>
+        <v>-0.2760401584447459</v>
       </c>
       <c r="P18">
-        <v>-0.2760401584447459</v>
+        <v>6.12072996601273</v>
       </c>
       <c r="Q18">
-        <v>6.12072996601273</v>
+        <v>1.709239506270284</v>
       </c>
       <c r="R18">
-        <v>1.709239506270284</v>
+        <v>0.6323788320998519</v>
       </c>
       <c r="S18">
-        <v>0.6323788320998519</v>
+        <v>1.73641277900912</v>
       </c>
       <c r="T18">
-        <v>1.73641277900912</v>
-      </c>
-      <c r="U18">
         <v>2.029123419250828</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -1375,57 +1336,54 @@
         <v>4.253858447199108</v>
       </c>
       <c r="F19">
-        <v>-0.5470286381063533</v>
+        <v>2.588102911237619</v>
       </c>
       <c r="G19">
-        <v>2.041074273131266</v>
+        <v>-0.1005341253553887</v>
       </c>
       <c r="H19">
-        <v>-0.1005341253553887</v>
+        <v>-12.51021640180594</v>
       </c>
       <c r="I19">
-        <v>-12.51021640180594</v>
+        <v>66.34507621989349</v>
       </c>
       <c r="J19">
-        <v>66.34507621989349</v>
+        <v>6.741638607124738</v>
       </c>
       <c r="K19">
-        <v>6.741638607124738</v>
+        <v>20.61853758327431</v>
       </c>
       <c r="L19">
-        <v>20.61853758327431</v>
+        <v>4.610747817834914</v>
       </c>
       <c r="M19">
-        <v>4.610747817834914</v>
+        <v>1.091689690429642</v>
       </c>
       <c r="N19">
-        <v>1.091689690429642</v>
+        <v>1.648396027496877</v>
       </c>
       <c r="O19">
-        <v>1.648396027496877</v>
+        <v>-0.272780692832646</v>
       </c>
       <c r="P19">
-        <v>-0.272780692832646</v>
+        <v>6.637078878833093</v>
       </c>
       <c r="Q19">
-        <v>6.637078878833093</v>
+        <v>-0.2889343605374137</v>
       </c>
       <c r="R19">
-        <v>-0.2889343605374137</v>
+        <v>0.6176177928355377</v>
       </c>
       <c r="S19">
-        <v>0.6176177928355377</v>
+        <v>1.570516968468718</v>
       </c>
       <c r="T19">
-        <v>1.570516968468718</v>
-      </c>
-      <c r="U19">
         <v>3.345266394421215</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>24</v>
@@ -1440,57 +1398,54 @@
         <v>2.990827620323336</v>
       </c>
       <c r="F20">
-        <v>-0.5400032315454714</v>
+        <v>2.268791010543967</v>
       </c>
       <c r="G20">
-        <v>1.728787778998496</v>
+        <v>-0.1028553219948377</v>
       </c>
       <c r="H20">
-        <v>-0.1028553219948377</v>
+        <v>-10.08632222445642</v>
       </c>
       <c r="I20">
-        <v>-10.08632222445642</v>
+        <v>50.48063600415131</v>
       </c>
       <c r="J20">
-        <v>50.48063600415131</v>
+        <v>7.560297923155022</v>
       </c>
       <c r="K20">
-        <v>7.560297923155022</v>
+        <v>8.000669240995975</v>
       </c>
       <c r="L20">
-        <v>8.000669240995975</v>
+        <v>3.109730312285321</v>
       </c>
       <c r="M20">
-        <v>3.109730312285321</v>
+        <v>1.508862368052527</v>
       </c>
       <c r="N20">
-        <v>1.508862368052527</v>
+        <v>1.744545868644762</v>
       </c>
       <c r="O20">
-        <v>1.744545868644762</v>
+        <v>-0.2142875422655715</v>
       </c>
       <c r="P20">
-        <v>-0.2142875422655715</v>
+        <v>5.562354186108506</v>
       </c>
       <c r="Q20">
-        <v>5.562354186108506</v>
+        <v>1.838887757120106</v>
       </c>
       <c r="R20">
-        <v>1.838887757120106</v>
+        <v>0.4898777672726335</v>
       </c>
       <c r="S20">
-        <v>0.4898777672726335</v>
+        <v>1.394654345218567</v>
       </c>
       <c r="T20">
-        <v>1.394654345218567</v>
-      </c>
-      <c r="U20">
         <v>4.193559593849103</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21">
         <v>24</v>
@@ -1505,57 +1460,54 @@
         <v>2.995789280216012</v>
       </c>
       <c r="F21">
-        <v>-0.5489293867190589</v>
+        <v>2.34093061538717</v>
       </c>
       <c r="G21">
-        <v>1.792001228668112</v>
+        <v>-0.09780455309500005</v>
       </c>
       <c r="H21">
-        <v>-0.09780455309500005</v>
+        <v>-10.2085835034783</v>
       </c>
       <c r="I21">
-        <v>-10.2085835034783</v>
+        <v>53.07377857667468</v>
       </c>
       <c r="J21">
-        <v>53.07377857667468</v>
+        <v>4.458429841090592</v>
       </c>
       <c r="K21">
-        <v>4.458429841090592</v>
+        <v>10.45999840012541</v>
       </c>
       <c r="L21">
-        <v>10.45999840012541</v>
+        <v>3.853998503445702</v>
       </c>
       <c r="M21">
-        <v>3.853998503445702</v>
+        <v>1.495668429862896</v>
       </c>
       <c r="N21">
-        <v>1.495668429862896</v>
+        <v>2.198270410555651</v>
       </c>
       <c r="O21">
-        <v>2.198270410555651</v>
+        <v>-0.2105533821138522</v>
       </c>
       <c r="P21">
-        <v>-0.2105533821138522</v>
+        <v>6.03208412292464</v>
       </c>
       <c r="Q21">
-        <v>6.03208412292464</v>
+        <v>2.75231295610355</v>
       </c>
       <c r="R21">
-        <v>2.75231295610355</v>
+        <v>0.573482305450614</v>
       </c>
       <c r="S21">
-        <v>0.573482305450614</v>
+        <v>1.967832259485043</v>
       </c>
       <c r="T21">
-        <v>1.967832259485043</v>
-      </c>
-      <c r="U21">
         <v>4.482205980410906</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>24</v>
@@ -1570,57 +1522,54 @@
         <v>2.833198365706635</v>
       </c>
       <c r="F22">
-        <v>-0.5627755449504557</v>
+        <v>2.137606490472667</v>
       </c>
       <c r="G22">
-        <v>1.574830945522211</v>
+        <v>-0.1107585091425637</v>
       </c>
       <c r="H22">
-        <v>-0.1107585091425637</v>
+        <v>-10.94024879637002</v>
       </c>
       <c r="I22">
-        <v>-10.94024879637002</v>
+        <v>48.93264263062832</v>
       </c>
       <c r="J22">
-        <v>48.93264263062832</v>
+        <v>3.878235676322087</v>
       </c>
       <c r="K22">
-        <v>3.878235676322087</v>
+        <v>10.66050392667031</v>
       </c>
       <c r="L22">
-        <v>10.66050392667031</v>
+        <v>2.962598477726053</v>
       </c>
       <c r="M22">
-        <v>2.962598477726053</v>
+        <v>1.225935727946515</v>
       </c>
       <c r="N22">
-        <v>1.225935727946515</v>
+        <v>1.474847298562026</v>
       </c>
       <c r="O22">
-        <v>1.474847298562026</v>
+        <v>-0.2143212801038563</v>
       </c>
       <c r="P22">
-        <v>-0.2143212801038563</v>
+        <v>5.269954133883139</v>
       </c>
       <c r="Q22">
-        <v>5.269954133883139</v>
+        <v>0.8774574781052474</v>
       </c>
       <c r="R22">
-        <v>0.8774574781052474</v>
+        <v>0.4437553097423738</v>
       </c>
       <c r="S22">
-        <v>0.4437553097423738</v>
+        <v>1.195961078826943</v>
       </c>
       <c r="T22">
-        <v>1.195961078826943</v>
-      </c>
-      <c r="U22">
         <v>3.656836479783097</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23">
         <v>24</v>
@@ -1635,57 +1584,54 @@
         <v>2.614032226632004</v>
       </c>
       <c r="F23">
-        <v>-0.5593603086605921</v>
+        <v>1.955318440522744</v>
       </c>
       <c r="G23">
-        <v>1.395958131862151</v>
+        <v>-0.1049094809948238</v>
       </c>
       <c r="H23">
-        <v>-0.1049094809948238</v>
+        <v>-10.23809910747236</v>
       </c>
       <c r="I23">
-        <v>-10.23809910747236</v>
+        <v>49.22059455135484</v>
       </c>
       <c r="J23">
-        <v>49.22059455135484</v>
+        <v>5.464662226115244</v>
       </c>
       <c r="K23">
-        <v>5.464662226115244</v>
+        <v>5.998993514679715</v>
       </c>
       <c r="L23">
-        <v>5.998993514679715</v>
+        <v>2.645567214590562</v>
       </c>
       <c r="M23">
-        <v>2.645567214590562</v>
+        <v>1.403962716759746</v>
       </c>
       <c r="N23">
-        <v>1.403962716759746</v>
+        <v>1.581064426480477</v>
       </c>
       <c r="O23">
-        <v>1.581064426480477</v>
+        <v>-0.2177001468345145</v>
       </c>
       <c r="P23">
-        <v>-0.2177001468345145</v>
+        <v>5.392380506208868</v>
       </c>
       <c r="Q23">
-        <v>5.392380506208868</v>
+        <v>1.302709197399536</v>
       </c>
       <c r="R23">
-        <v>1.302709197399536</v>
+        <v>0.4729990928233074</v>
       </c>
       <c r="S23">
-        <v>0.4729990928233074</v>
+        <v>1.481643547292985</v>
       </c>
       <c r="T23">
-        <v>1.481643547292985</v>
-      </c>
-      <c r="U23">
         <v>4.477917112856943</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <v>24</v>
@@ -1700,57 +1646,54 @@
         <v>2.958754614232115</v>
       </c>
       <c r="F24">
-        <v>-0.5510828190931236</v>
+        <v>2.057154078031326</v>
       </c>
       <c r="G24">
-        <v>1.506071258938202</v>
+        <v>-0.1204199275005222</v>
       </c>
       <c r="H24">
-        <v>-0.1204199275005222</v>
+        <v>-10.49625866911031</v>
       </c>
       <c r="I24">
-        <v>-10.49625866911031</v>
+        <v>50.99215522755635</v>
       </c>
       <c r="J24">
-        <v>50.99215522755635</v>
+        <v>11.91368206303982</v>
       </c>
       <c r="K24">
-        <v>11.91368206303982</v>
+        <v>4.070787575005669</v>
       </c>
       <c r="L24">
-        <v>4.070787575005669</v>
+        <v>3.057884246434268</v>
       </c>
       <c r="M24">
-        <v>3.057884246434268</v>
+        <v>1.424558137125393</v>
       </c>
       <c r="N24">
-        <v>1.424558137125393</v>
+        <v>1.735242619350075</v>
       </c>
       <c r="O24">
-        <v>1.735242619350075</v>
+        <v>-0.233571578232206</v>
       </c>
       <c r="P24">
-        <v>-0.233571578232206</v>
+        <v>5.341035000752142</v>
       </c>
       <c r="Q24">
-        <v>5.341035000752142</v>
+        <v>1.841185079352609</v>
       </c>
       <c r="R24">
-        <v>1.841185079352609</v>
+        <v>0.4832345804487516</v>
       </c>
       <c r="S24">
-        <v>0.4832345804487516</v>
+        <v>1.478644207452919</v>
       </c>
       <c r="T24">
-        <v>1.478644207452919</v>
-      </c>
-      <c r="U24">
         <v>3.772521896158369</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -1765,51 +1708,48 @@
         <v>2.894481900960319</v>
       </c>
       <c r="F25">
-        <v>-0.5520059159103101</v>
+        <v>2.142724429855566</v>
       </c>
       <c r="G25">
-        <v>1.590718513945256</v>
+        <v>-0.1196169259430157</v>
       </c>
       <c r="H25">
-        <v>-0.1196169259430157</v>
+        <v>-11.19677086928342</v>
       </c>
       <c r="I25">
-        <v>-11.19677086928342</v>
+        <v>49.91884149447154</v>
       </c>
       <c r="J25">
-        <v>49.91884149447154</v>
+        <v>6.440704493258846</v>
       </c>
       <c r="K25">
-        <v>6.440704493258846</v>
+        <v>11.00209456150866</v>
       </c>
       <c r="L25">
-        <v>11.00209456150866</v>
+        <v>2.419042068722978</v>
       </c>
       <c r="M25">
-        <v>2.419042068722978</v>
+        <v>1.415195793932482</v>
       </c>
       <c r="N25">
-        <v>1.415195793932482</v>
+        <v>1.652842239003918</v>
       </c>
       <c r="O25">
-        <v>1.652842239003918</v>
+        <v>-0.2132454420132467</v>
       </c>
       <c r="P25">
-        <v>-0.2132454420132467</v>
+        <v>5.676866141329301</v>
       </c>
       <c r="Q25">
-        <v>5.676866141329301</v>
+        <v>0.7431891486540417</v>
       </c>
       <c r="R25">
-        <v>0.7431891486540417</v>
+        <v>0.527357910082755</v>
       </c>
       <c r="S25">
-        <v>0.527357910082755</v>
+        <v>1.625669671638496</v>
       </c>
       <c r="T25">
-        <v>1.625669671638496</v>
-      </c>
-      <c r="U25">
         <v>4.393942024791499</v>
       </c>
     </row>

</xml_diff>